<commit_message>
Updated Cantenna Characterization Spreadsheet.
</commit_message>
<xml_diff>
--- a/Final Project/Team 1/Team1FullRSSIdata.xlsx
+++ b/Final Project/Team 1/Team1FullRSSIdata.xlsx
@@ -57,9 +57,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,8 +380,7 @@
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H3,4,FALSE)+23</f>
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
@@ -390,8 +388,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H4,4,FALSE)+23</f>
+      <c r="B4">
         <v>0</v>
       </c>
     </row>
@@ -399,8 +396,7 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H5,4,FALSE)+23</f>
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
@@ -408,8 +404,7 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H6,4,FALSE)+23</f>
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
@@ -417,8 +412,7 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H7,4,FALSE)+23</f>
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
@@ -426,8 +420,7 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H8,4,FALSE)+23</f>
+      <c r="B8">
         <v>0</v>
       </c>
     </row>
@@ -435,8 +428,7 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H9,4,FALSE)+23</f>
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
@@ -444,8 +436,7 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H10,4,FALSE)+23</f>
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
@@ -453,8 +444,7 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H11,4,FALSE)+23</f>
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
@@ -462,8 +452,7 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H12,4,FALSE)+23</f>
+      <c r="B12">
         <v>0</v>
       </c>
     </row>
@@ -471,8 +460,7 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H13,4,FALSE)+23</f>
+      <c r="B13">
         <v>0</v>
       </c>
     </row>
@@ -480,8 +468,7 @@
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H14,4,FALSE)+23</f>
+      <c r="B14">
         <v>-3.2000000000000028E-2</v>
       </c>
     </row>
@@ -489,8 +476,7 @@
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H15,4,FALSE)+23</f>
+      <c r="B15">
         <v>-0.12266666666666737</v>
       </c>
     </row>
@@ -498,8 +484,7 @@
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H16,4,FALSE)+23</f>
+      <c r="B16">
         <v>-0.26399999999999935</v>
       </c>
     </row>
@@ -507,8 +492,7 @@
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H17,4,FALSE)+23</f>
+      <c r="B17">
         <v>-0.4480000000000004</v>
       </c>
     </row>
@@ -516,8 +500,7 @@
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H18,4,FALSE)+23</f>
+      <c r="B18">
         <v>-0.66666666666666785</v>
       </c>
     </row>
@@ -525,8 +508,7 @@
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H19,4,FALSE)+23</f>
+      <c r="B19">
         <v>-0.91199999999999903</v>
       </c>
     </row>
@@ -534,8 +516,7 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H20,4,FALSE)+23</f>
+      <c r="B20">
         <v>-1.1760000000000019</v>
       </c>
     </row>
@@ -543,8 +524,7 @@
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H21,4,FALSE)+23</f>
+      <c r="B21">
         <v>-1.4506666666666668</v>
       </c>
     </row>
@@ -552,8 +532,7 @@
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H22,4,FALSE)+23</f>
+      <c r="B22">
         <v>-1.7280000000000015</v>
       </c>
     </row>
@@ -561,8 +540,7 @@
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H23,4,FALSE)+23</f>
+      <c r="B23">
         <v>-2</v>
       </c>
     </row>
@@ -570,8 +548,7 @@
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H24,4,FALSE)+23</f>
+      <c r="B24">
         <v>-2.3279999999999994</v>
       </c>
     </row>
@@ -579,8 +556,7 @@
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H25,4,FALSE)+23</f>
+      <c r="B25">
         <v>-2.7573333333333352</v>
       </c>
     </row>
@@ -588,8 +564,7 @@
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H26,4,FALSE)+23</f>
+      <c r="B26">
         <v>-3.2560000000000002</v>
       </c>
     </row>
@@ -597,8 +572,7 @@
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H27,4,FALSE)+23</f>
+      <c r="B27">
         <v>-3.7920000000000016</v>
       </c>
     </row>
@@ -606,8 +580,7 @@
       <c r="A28">
         <v>25</v>
       </c>
-      <c r="B28" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H28,4,FALSE)+23</f>
+      <c r="B28">
         <v>-4.3333333333333321</v>
       </c>
     </row>
@@ -615,8 +588,7 @@
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H29,4,FALSE)+23</f>
+      <c r="B29">
         <v>-4.847999999999999</v>
       </c>
     </row>
@@ -624,8 +596,7 @@
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H30,4,FALSE)+23</f>
+      <c r="B30">
         <v>-5.304000000000002</v>
       </c>
     </row>
@@ -633,8 +604,7 @@
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H31,4,FALSE)+23</f>
+      <c r="B31">
         <v>-5.6693333333333342</v>
       </c>
     </row>
@@ -642,8 +612,7 @@
       <c r="A32">
         <v>29</v>
       </c>
-      <c r="B32" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H32,4,FALSE)+23</f>
+      <c r="B32">
         <v>-5.911999999999999</v>
       </c>
     </row>
@@ -651,8 +620,7 @@
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H33,4,FALSE)+23</f>
+      <c r="B33">
         <v>-6</v>
       </c>
     </row>
@@ -660,8 +628,7 @@
       <c r="A34">
         <v>31</v>
       </c>
-      <c r="B34" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H34,4,FALSE)+23</f>
+      <c r="B34">
         <v>-6</v>
       </c>
     </row>
@@ -669,8 +636,7 @@
       <c r="A35">
         <v>32</v>
       </c>
-      <c r="B35" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H35,4,FALSE)+23</f>
+      <c r="B35">
         <v>-6</v>
       </c>
     </row>
@@ -678,8 +644,7 @@
       <c r="A36">
         <v>33</v>
       </c>
-      <c r="B36" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H36,4,FALSE)+23</f>
+      <c r="B36">
         <v>-6</v>
       </c>
     </row>
@@ -687,8 +652,7 @@
       <c r="A37">
         <v>34</v>
       </c>
-      <c r="B37" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H37,4,FALSE)+23</f>
+      <c r="B37">
         <v>-6</v>
       </c>
     </row>
@@ -696,8 +660,7 @@
       <c r="A38">
         <v>35</v>
       </c>
-      <c r="B38" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H38,4,FALSE)+23</f>
+      <c r="B38">
         <v>-6</v>
       </c>
     </row>
@@ -705,8 +668,7 @@
       <c r="A39">
         <v>36</v>
       </c>
-      <c r="B39" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H39,4,FALSE)+23</f>
+      <c r="B39">
         <v>-6</v>
       </c>
     </row>
@@ -714,8 +676,7 @@
       <c r="A40">
         <v>37</v>
       </c>
-      <c r="B40" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H40,4,FALSE)+23</f>
+      <c r="B40">
         <v>-6</v>
       </c>
     </row>
@@ -723,8 +684,7 @@
       <c r="A41">
         <v>38</v>
       </c>
-      <c r="B41" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H41,4,FALSE)+23</f>
+      <c r="B41">
         <v>-6</v>
       </c>
     </row>
@@ -732,8 +692,7 @@
       <c r="A42">
         <v>39</v>
       </c>
-      <c r="B42" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H42,4,FALSE)+23</f>
+      <c r="B42">
         <v>-6</v>
       </c>
     </row>
@@ -741,8 +700,7 @@
       <c r="A43">
         <v>40</v>
       </c>
-      <c r="B43" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H43,4,FALSE)+23</f>
+      <c r="B43">
         <v>-6</v>
       </c>
     </row>
@@ -750,8 +708,7 @@
       <c r="A44">
         <v>41</v>
       </c>
-      <c r="B44" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H44,4,FALSE)+23</f>
+      <c r="B44">
         <v>-6.0380000000000003</v>
       </c>
     </row>
@@ -759,8 +716,7 @@
       <c r="A45">
         <v>42</v>
       </c>
-      <c r="B45" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H45,4,FALSE)+23</f>
+      <c r="B45">
         <v>-6.1439999999999984</v>
       </c>
     </row>
@@ -768,8 +724,7 @@
       <c r="A46">
         <v>43</v>
       </c>
-      <c r="B46" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H46,4,FALSE)+23</f>
+      <c r="B46">
         <v>-6.3060000000000009</v>
       </c>
     </row>
@@ -777,8 +732,7 @@
       <c r="A47">
         <v>44</v>
       </c>
-      <c r="B47" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H47,4,FALSE)+23</f>
+      <c r="B47">
         <v>-6.5120000000000005</v>
       </c>
     </row>
@@ -786,8 +740,7 @@
       <c r="A48">
         <v>45</v>
       </c>
-      <c r="B48" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H48,4,FALSE)+23</f>
+      <c r="B48">
         <v>-6.75</v>
       </c>
     </row>
@@ -795,8 +748,7 @@
       <c r="A49">
         <v>46</v>
       </c>
-      <c r="B49" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H49,4,FALSE)+23</f>
+      <c r="B49">
         <v>-7.0079999999999991</v>
       </c>
     </row>
@@ -804,8 +756,7 @@
       <c r="A50">
         <v>47</v>
       </c>
-      <c r="B50" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H50,4,FALSE)+23</f>
+      <c r="B50">
         <v>-7.2740000000000009</v>
       </c>
     </row>
@@ -813,8 +764,7 @@
       <c r="A51">
         <v>48</v>
       </c>
-      <c r="B51" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H51,4,FALSE)+23</f>
+      <c r="B51">
         <v>-7.5360000000000014</v>
       </c>
     </row>
@@ -822,8 +772,7 @@
       <c r="A52">
         <v>49</v>
       </c>
-      <c r="B52" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H52,4,FALSE)+23</f>
+      <c r="B52">
         <v>-7.782</v>
       </c>
     </row>
@@ -831,8 +780,7 @@
       <c r="A53">
         <v>50</v>
       </c>
-      <c r="B53" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H53,4,FALSE)+23</f>
+      <c r="B53">
         <v>-8</v>
       </c>
     </row>
@@ -840,8 +788,7 @@
       <c r="A54">
         <v>51</v>
       </c>
-      <c r="B54" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H54,4,FALSE)+23</f>
+      <c r="B54">
         <v>-8.1999999999999993</v>
       </c>
     </row>
@@ -849,8 +796,7 @@
       <c r="A55">
         <v>52</v>
       </c>
-      <c r="B55" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H55,4,FALSE)+23</f>
+      <c r="B55">
         <v>-8.3999999999999986</v>
       </c>
     </row>
@@ -858,8 +804,7 @@
       <c r="A56">
         <v>53</v>
       </c>
-      <c r="B56" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H56,4,FALSE)+23</f>
+      <c r="B56">
         <v>-8.6000000000000014</v>
       </c>
     </row>
@@ -867,8 +812,7 @@
       <c r="A57">
         <v>54</v>
       </c>
-      <c r="B57" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H57,4,FALSE)+23</f>
+      <c r="B57">
         <v>-8.8000000000000007</v>
       </c>
     </row>
@@ -876,8 +820,7 @@
       <c r="A58">
         <v>55</v>
       </c>
-      <c r="B58" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H58,4,FALSE)+23</f>
+      <c r="B58">
         <v>-9</v>
       </c>
     </row>
@@ -885,8 +828,7 @@
       <c r="A59">
         <v>56</v>
       </c>
-      <c r="B59" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H59,4,FALSE)+23</f>
+      <c r="B59">
         <v>-9.2000000000000028</v>
       </c>
     </row>
@@ -894,8 +836,7 @@
       <c r="A60">
         <v>57</v>
       </c>
-      <c r="B60" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H60,4,FALSE)+23</f>
+      <c r="B60">
         <v>-9.3999999999999986</v>
       </c>
     </row>
@@ -903,8 +844,7 @@
       <c r="A61">
         <v>58</v>
       </c>
-      <c r="B61" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H61,4,FALSE)+23</f>
+      <c r="B61">
         <v>-9.6000000000000014</v>
       </c>
     </row>
@@ -912,8 +852,7 @@
       <c r="A62">
         <v>59</v>
       </c>
-      <c r="B62" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H62,4,FALSE)+23</f>
+      <c r="B62">
         <v>-9.7999999999999972</v>
       </c>
     </row>
@@ -921,8 +860,7 @@
       <c r="A63">
         <v>60</v>
       </c>
-      <c r="B63" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H63,4,FALSE)+23</f>
+      <c r="B63">
         <v>-10</v>
       </c>
     </row>
@@ -930,8 +868,7 @@
       <c r="A64">
         <v>61</v>
       </c>
-      <c r="B64" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H64,4,FALSE)+23</f>
+      <c r="B64">
         <v>-10.200000000000003</v>
       </c>
     </row>
@@ -939,8 +876,7 @@
       <c r="A65">
         <v>62</v>
       </c>
-      <c r="B65" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H65,4,FALSE)+23</f>
+      <c r="B65">
         <v>-10.399999999999999</v>
       </c>
     </row>
@@ -948,8 +884,7 @@
       <c r="A66">
         <v>63</v>
       </c>
-      <c r="B66" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H66,4,FALSE)+23</f>
+      <c r="B66">
         <v>-10.600000000000001</v>
       </c>
     </row>
@@ -957,8 +892,7 @@
       <c r="A67">
         <v>64</v>
       </c>
-      <c r="B67" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H67,4,FALSE)+23</f>
+      <c r="B67">
         <v>-10.799999999999997</v>
       </c>
     </row>
@@ -966,8 +900,7 @@
       <c r="A68">
         <v>65</v>
       </c>
-      <c r="B68" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H68,4,FALSE)+23</f>
+      <c r="B68">
         <v>-11</v>
       </c>
     </row>
@@ -975,8 +908,7 @@
       <c r="A69">
         <v>66</v>
       </c>
-      <c r="B69" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H69,4,FALSE)+23</f>
+      <c r="B69">
         <v>-11.200000000000003</v>
       </c>
     </row>
@@ -984,8 +916,7 @@
       <c r="A70">
         <v>67</v>
       </c>
-      <c r="B70" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H70,4,FALSE)+23</f>
+      <c r="B70">
         <v>-11.399999999999999</v>
       </c>
     </row>
@@ -993,8 +924,7 @@
       <c r="A71">
         <v>68</v>
       </c>
-      <c r="B71" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H71,4,FALSE)+23</f>
+      <c r="B71">
         <v>-11.600000000000001</v>
       </c>
     </row>
@@ -1002,8 +932,7 @@
       <c r="A72">
         <v>69</v>
       </c>
-      <c r="B72" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H72,4,FALSE)+23</f>
+      <c r="B72">
         <v>-11.799999999999997</v>
       </c>
     </row>
@@ -1011,8 +940,7 @@
       <c r="A73">
         <v>70</v>
       </c>
-      <c r="B73" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H73,4,FALSE)+23</f>
+      <c r="B73">
         <v>-12</v>
       </c>
     </row>
@@ -1020,8 +948,7 @@
       <c r="A74">
         <v>71</v>
       </c>
-      <c r="B74" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H74,4,FALSE)+23</f>
+      <c r="B74">
         <v>-12.194000000000003</v>
       </c>
     </row>
@@ -1029,8 +956,7 @@
       <c r="A75">
         <v>72</v>
       </c>
-      <c r="B75" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H75,4,FALSE)+23</f>
+      <c r="B75">
         <v>-12.378666666666668</v>
       </c>
     </row>
@@ -1038,8 +964,7 @@
       <c r="A76">
         <v>73</v>
       </c>
-      <c r="B76" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H76,4,FALSE)+23</f>
+      <c r="B76">
         <v>-12.558</v>
       </c>
     </row>
@@ -1047,8 +972,7 @@
       <c r="A77">
         <v>74</v>
       </c>
-      <c r="B77" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H77,4,FALSE)+23</f>
+      <c r="B77">
         <v>-12.735999999999997</v>
       </c>
     </row>
@@ -1056,8 +980,7 @@
       <c r="A78">
         <v>75</v>
       </c>
-      <c r="B78" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H78,4,FALSE)+23</f>
+      <c r="B78">
         <v>-12.916666666666664</v>
       </c>
     </row>
@@ -1065,8 +988,7 @@
       <c r="A79">
         <v>76</v>
       </c>
-      <c r="B79" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H79,4,FALSE)+23</f>
+      <c r="B79">
         <v>-13.103999999999999</v>
       </c>
     </row>
@@ -1074,8 +996,7 @@
       <c r="A80">
         <v>77</v>
       </c>
-      <c r="B80" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H80,4,FALSE)+23</f>
+      <c r="B80">
         <v>-13.302</v>
       </c>
     </row>
@@ -1083,8 +1004,7 @@
       <c r="A81">
         <v>78</v>
       </c>
-      <c r="B81" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H81,4,FALSE)+23</f>
+      <c r="B81">
         <v>-13.51466666666667</v>
       </c>
     </row>
@@ -1092,8 +1012,7 @@
       <c r="A82">
         <v>79</v>
       </c>
-      <c r="B82" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H82,4,FALSE)+23</f>
+      <c r="B82">
         <v>-13.746000000000002</v>
       </c>
     </row>
@@ -1101,8 +1020,7 @@
       <c r="A83">
         <v>80</v>
       </c>
-      <c r="B83" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H83,4,FALSE)+23</f>
+      <c r="B83">
         <v>-14</v>
       </c>
     </row>
@@ -1110,8 +1028,7 @@
       <c r="A84">
         <v>81</v>
       </c>
-      <c r="B84" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H84,4,FALSE)+23</f>
+      <c r="B84">
         <v>-14.304000000000002</v>
       </c>
     </row>
@@ -1119,8 +1036,7 @@
       <c r="A85">
         <v>82</v>
       </c>
-      <c r="B85" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H85,4,FALSE)+23</f>
+      <c r="B85">
         <v>-14.671999999999997</v>
       </c>
     </row>
@@ -1128,8 +1044,7 @@
       <c r="A86">
         <v>83</v>
       </c>
-      <c r="B86" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H86,4,FALSE)+23</f>
+      <c r="B86">
         <v>-15.088000000000001</v>
       </c>
     </row>
@@ -1137,8 +1052,7 @@
       <c r="A87">
         <v>84</v>
       </c>
-      <c r="B87" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H87,4,FALSE)+23</f>
+      <c r="B87">
         <v>-15.536000000000001</v>
       </c>
     </row>
@@ -1146,8 +1060,7 @@
       <c r="A88">
         <v>85</v>
       </c>
-      <c r="B88" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H88,4,FALSE)+23</f>
+      <c r="B88">
         <v>-16</v>
       </c>
     </row>
@@ -1155,8 +1068,7 @@
       <c r="A89">
         <v>86</v>
       </c>
-      <c r="B89" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H89,4,FALSE)+23</f>
+      <c r="B89">
         <v>-16.463999999999999</v>
       </c>
     </row>
@@ -1164,8 +1076,7 @@
       <c r="A90">
         <v>87</v>
       </c>
-      <c r="B90" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H90,4,FALSE)+23</f>
+      <c r="B90">
         <v>-16.911999999999999</v>
       </c>
     </row>
@@ -1173,8 +1084,7 @@
       <c r="A91">
         <v>88</v>
       </c>
-      <c r="B91" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H91,4,FALSE)+23</f>
+      <c r="B91">
         <v>-17.328000000000003</v>
       </c>
     </row>
@@ -1182,8 +1092,7 @@
       <c r="A92">
         <v>89</v>
       </c>
-      <c r="B92" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H92,4,FALSE)+23</f>
+      <c r="B92">
         <v>-17.695999999999998</v>
       </c>
     </row>
@@ -1191,8 +1100,7 @@
       <c r="A93">
         <v>90</v>
       </c>
-      <c r="B93" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H93,4,FALSE)+23</f>
+      <c r="B93">
         <v>-18</v>
       </c>
     </row>
@@ -1200,8 +1108,7 @@
       <c r="A94">
         <v>91</v>
       </c>
-      <c r="B94" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H94,4,FALSE)+23</f>
+      <c r="B94">
         <v>-18.271999999999998</v>
       </c>
     </row>
@@ -1209,8 +1116,7 @@
       <c r="A95">
         <v>92</v>
       </c>
-      <c r="B95" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H95,4,FALSE)+23</f>
+      <c r="B95">
         <v>-18.549333333333337</v>
       </c>
     </row>
@@ -1218,8 +1124,7 @@
       <c r="A96">
         <v>93</v>
       </c>
-      <c r="B96" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H96,4,FALSE)+23</f>
+      <c r="B96">
         <v>-18.823999999999998</v>
       </c>
     </row>
@@ -1227,8 +1132,7 @@
       <c r="A97">
         <v>94</v>
       </c>
-      <c r="B97" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H97,4,FALSE)+23</f>
+      <c r="B97">
         <v>-19.088000000000001</v>
       </c>
     </row>
@@ -1236,8 +1140,7 @@
       <c r="A98">
         <v>95</v>
       </c>
-      <c r="B98" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H98,4,FALSE)+23</f>
+      <c r="B98">
         <v>-19.333333333333336</v>
       </c>
     </row>
@@ -1245,8 +1148,7 @@
       <c r="A99">
         <v>96</v>
       </c>
-      <c r="B99" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H99,4,FALSE)+23</f>
+      <c r="B99">
         <v>-19.552</v>
       </c>
     </row>
@@ -1254,8 +1156,7 @@
       <c r="A100">
         <v>97</v>
       </c>
-      <c r="B100" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H100,4,FALSE)+23</f>
+      <c r="B100">
         <v>-19.735999999999997</v>
       </c>
     </row>
@@ -1263,8 +1164,7 @@
       <c r="A101">
         <v>98</v>
       </c>
-      <c r="B101" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H101,4,FALSE)+23</f>
+      <c r="B101">
         <v>-19.877333333333333</v>
       </c>
     </row>
@@ -1272,8 +1172,7 @@
       <c r="A102">
         <v>99</v>
       </c>
-      <c r="B102" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H102,4,FALSE)+23</f>
+      <c r="B102">
         <v>-19.968000000000004</v>
       </c>
     </row>
@@ -1281,8 +1180,7 @@
       <c r="A103">
         <v>100</v>
       </c>
-      <c r="B103" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H103,4,FALSE)+23</f>
+      <c r="B103">
         <v>-20</v>
       </c>
     </row>
@@ -1290,8 +1188,7 @@
       <c r="A104">
         <v>101</v>
       </c>
-      <c r="B104" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H104,4,FALSE)+23</f>
+      <c r="B104">
         <v>-19.832000000000001</v>
       </c>
     </row>
@@ -1299,8 +1196,7 @@
       <c r="A105">
         <v>102</v>
       </c>
-      <c r="B105" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H105,4,FALSE)+23</f>
+      <c r="B105">
         <v>-19.375999999999998</v>
       </c>
     </row>
@@ -1308,8 +1204,7 @@
       <c r="A106">
         <v>103</v>
       </c>
-      <c r="B106" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H106,4,FALSE)+23</f>
+      <c r="B106">
         <v>-18.704000000000001</v>
       </c>
     </row>
@@ -1317,8 +1212,7 @@
       <c r="A107">
         <v>104</v>
       </c>
-      <c r="B107" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H107,4,FALSE)+23</f>
+      <c r="B107">
         <v>-17.887999999999998</v>
       </c>
     </row>
@@ -1326,8 +1220,7 @@
       <c r="A108">
         <v>105</v>
       </c>
-      <c r="B108" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H108,4,FALSE)+23</f>
+      <c r="B108">
         <v>-17</v>
       </c>
     </row>
@@ -1335,8 +1228,7 @@
       <c r="A109">
         <v>106</v>
       </c>
-      <c r="B109" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H109,4,FALSE)+23</f>
+      <c r="B109">
         <v>-16.112000000000002</v>
       </c>
     </row>
@@ -1344,8 +1236,7 @@
       <c r="A110">
         <v>107</v>
       </c>
-      <c r="B110" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H110,4,FALSE)+23</f>
+      <c r="B110">
         <v>-15.295999999999999</v>
       </c>
     </row>
@@ -1353,8 +1244,7 @@
       <c r="A111">
         <v>108</v>
       </c>
-      <c r="B111" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H111,4,FALSE)+23</f>
+      <c r="B111">
         <v>-14.624000000000002</v>
       </c>
     </row>
@@ -1362,8 +1252,7 @@
       <c r="A112">
         <v>109</v>
       </c>
-      <c r="B112" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H112,4,FALSE)+23</f>
+      <c r="B112">
         <v>-14.167999999999999</v>
       </c>
     </row>
@@ -1371,8 +1260,7 @@
       <c r="A113">
         <v>110</v>
       </c>
-      <c r="B113" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H113,4,FALSE)+23</f>
+      <c r="B113">
         <v>-14</v>
       </c>
     </row>
@@ -1380,8 +1268,7 @@
       <c r="A114">
         <v>111</v>
       </c>
-      <c r="B114" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H114,4,FALSE)+23</f>
+      <c r="B114">
         <v>-14.055999999999997</v>
       </c>
     </row>
@@ -1389,8 +1276,7 @@
       <c r="A115">
         <v>112</v>
       </c>
-      <c r="B115" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H115,4,FALSE)+23</f>
+      <c r="B115">
         <v>-14.207999999999998</v>
       </c>
     </row>
@@ -1398,8 +1284,7 @@
       <c r="A116">
         <v>113</v>
       </c>
-      <c r="B116" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H116,4,FALSE)+23</f>
+      <c r="B116">
         <v>-14.432000000000002</v>
       </c>
     </row>
@@ -1407,8 +1292,7 @@
       <c r="A117">
         <v>114</v>
       </c>
-      <c r="B117" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H117,4,FALSE)+23</f>
+      <c r="B117">
         <v>-14.704000000000001</v>
       </c>
     </row>
@@ -1416,8 +1300,7 @@
       <c r="A118">
         <v>115</v>
       </c>
-      <c r="B118" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H118,4,FALSE)+23</f>
+      <c r="B118">
         <v>-15</v>
       </c>
     </row>
@@ -1425,8 +1308,7 @@
       <c r="A119">
         <v>116</v>
       </c>
-      <c r="B119" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H119,4,FALSE)+23</f>
+      <c r="B119">
         <v>-15.295999999999999</v>
       </c>
     </row>
@@ -1434,8 +1316,7 @@
       <c r="A120">
         <v>117</v>
       </c>
-      <c r="B120" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H120,4,FALSE)+23</f>
+      <c r="B120">
         <v>-15.567999999999998</v>
       </c>
     </row>
@@ -1443,8 +1324,7 @@
       <c r="A121">
         <v>118</v>
       </c>
-      <c r="B121" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H121,4,FALSE)+23</f>
+      <c r="B121">
         <v>-15.792000000000002</v>
       </c>
     </row>
@@ -1452,8 +1332,7 @@
       <c r="A122">
         <v>119</v>
       </c>
-      <c r="B122" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H122,4,FALSE)+23</f>
+      <c r="B122">
         <v>-15.944000000000003</v>
       </c>
     </row>
@@ -1461,8 +1340,7 @@
       <c r="A123">
         <v>120</v>
       </c>
-      <c r="B123" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H123,4,FALSE)+23</f>
+      <c r="B123">
         <v>-16</v>
       </c>
     </row>
@@ -1470,8 +1348,7 @@
       <c r="A124">
         <v>121</v>
       </c>
-      <c r="B124" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H124,4,FALSE)+23</f>
+      <c r="B124">
         <v>-15.944000000000003</v>
       </c>
     </row>
@@ -1479,8 +1356,7 @@
       <c r="A125">
         <v>122</v>
       </c>
-      <c r="B125" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H125,4,FALSE)+23</f>
+      <c r="B125">
         <v>-15.792000000000002</v>
       </c>
     </row>
@@ -1488,8 +1364,7 @@
       <c r="A126">
         <v>123</v>
       </c>
-      <c r="B126" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H126,4,FALSE)+23</f>
+      <c r="B126">
         <v>-15.567999999999998</v>
       </c>
     </row>
@@ -1497,8 +1372,7 @@
       <c r="A127">
         <v>124</v>
       </c>
-      <c r="B127" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H127,4,FALSE)+23</f>
+      <c r="B127">
         <v>-15.295999999999999</v>
       </c>
     </row>
@@ -1506,8 +1380,7 @@
       <c r="A128">
         <v>125</v>
       </c>
-      <c r="B128" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H128,4,FALSE)+23</f>
+      <c r="B128">
         <v>-15</v>
       </c>
     </row>
@@ -1515,8 +1388,7 @@
       <c r="A129">
         <v>126</v>
       </c>
-      <c r="B129" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H129,4,FALSE)+23</f>
+      <c r="B129">
         <v>-14.704000000000001</v>
       </c>
     </row>
@@ -1524,8 +1396,7 @@
       <c r="A130">
         <v>127</v>
       </c>
-      <c r="B130" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H130,4,FALSE)+23</f>
+      <c r="B130">
         <v>-14.432000000000002</v>
       </c>
     </row>
@@ -1533,8 +1404,7 @@
       <c r="A131">
         <v>128</v>
       </c>
-      <c r="B131" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H131,4,FALSE)+23</f>
+      <c r="B131">
         <v>-14.207999999999998</v>
       </c>
     </row>
@@ -1542,8 +1412,7 @@
       <c r="A132">
         <v>129</v>
       </c>
-      <c r="B132" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H132,4,FALSE)+23</f>
+      <c r="B132">
         <v>-14.055999999999997</v>
       </c>
     </row>
@@ -1551,8 +1420,7 @@
       <c r="A133">
         <v>130</v>
       </c>
-      <c r="B133" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H133,4,FALSE)+23</f>
+      <c r="B133">
         <v>-14</v>
       </c>
     </row>
@@ -1560,8 +1428,7 @@
       <c r="A134">
         <v>131</v>
       </c>
-      <c r="B134" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H134,4,FALSE)+23</f>
+      <c r="B134">
         <v>-14.037999999999997</v>
       </c>
     </row>
@@ -1569,8 +1436,7 @@
       <c r="A135">
         <v>132</v>
       </c>
-      <c r="B135" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H135,4,FALSE)+23</f>
+      <c r="B135">
         <v>-14.143999999999998</v>
       </c>
     </row>
@@ -1578,8 +1444,7 @@
       <c r="A136">
         <v>133</v>
       </c>
-      <c r="B136" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H136,4,FALSE)+23</f>
+      <c r="B136">
         <v>-14.305999999999997</v>
       </c>
     </row>
@@ -1587,8 +1452,7 @@
       <c r="A137">
         <v>134</v>
       </c>
-      <c r="B137" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H137,4,FALSE)+23</f>
+      <c r="B137">
         <v>-14.512</v>
       </c>
     </row>
@@ -1596,8 +1460,7 @@
       <c r="A138">
         <v>135</v>
       </c>
-      <c r="B138" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H138,4,FALSE)+23</f>
+      <c r="B138">
         <v>-14.75</v>
       </c>
     </row>
@@ -1605,8 +1468,7 @@
       <c r="A139">
         <v>136</v>
       </c>
-      <c r="B139" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H139,4,FALSE)+23</f>
+      <c r="B139">
         <v>-15.008000000000003</v>
       </c>
     </row>
@@ -1614,8 +1476,7 @@
       <c r="A140">
         <v>137</v>
       </c>
-      <c r="B140" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H140,4,FALSE)+23</f>
+      <c r="B140">
         <v>-15.274000000000001</v>
       </c>
     </row>
@@ -1623,8 +1484,7 @@
       <c r="A141">
         <v>138</v>
       </c>
-      <c r="B141" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H141,4,FALSE)+23</f>
+      <c r="B141">
         <v>-15.536000000000001</v>
       </c>
     </row>
@@ -1632,8 +1492,7 @@
       <c r="A142">
         <v>139</v>
       </c>
-      <c r="B142" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H142,4,FALSE)+23</f>
+      <c r="B142">
         <v>-15.782000000000004</v>
       </c>
     </row>
@@ -1641,8 +1500,7 @@
       <c r="A143">
         <v>140</v>
       </c>
-      <c r="B143" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H143,4,FALSE)+23</f>
+      <c r="B143">
         <v>-16</v>
       </c>
     </row>
@@ -1650,8 +1508,7 @@
       <c r="A144">
         <v>141</v>
       </c>
-      <c r="B144" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H144,4,FALSE)+23</f>
+      <c r="B144">
         <v>-16.218000000000004</v>
       </c>
     </row>
@@ -1659,8 +1516,7 @@
       <c r="A145">
         <v>142</v>
       </c>
-      <c r="B145" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H145,4,FALSE)+23</f>
+      <c r="B145">
         <v>-16.463999999999999</v>
       </c>
     </row>
@@ -1668,8 +1524,7 @@
       <c r="A146">
         <v>143</v>
       </c>
-      <c r="B146" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H146,4,FALSE)+23</f>
+      <c r="B146">
         <v>-16.725999999999999</v>
       </c>
     </row>
@@ -1677,8 +1532,7 @@
       <c r="A147">
         <v>144</v>
       </c>
-      <c r="B147" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H147,4,FALSE)+23</f>
+      <c r="B147">
         <v>-16.991999999999997</v>
       </c>
     </row>
@@ -1686,8 +1540,7 @@
       <c r="A148">
         <v>145</v>
       </c>
-      <c r="B148" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H148,4,FALSE)+23</f>
+      <c r="B148">
         <v>-17.25</v>
       </c>
     </row>
@@ -1695,8 +1548,7 @@
       <c r="A149">
         <v>146</v>
       </c>
-      <c r="B149" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H149,4,FALSE)+23</f>
+      <c r="B149">
         <v>-17.488</v>
       </c>
     </row>
@@ -1704,8 +1556,7 @@
       <c r="A150">
         <v>147</v>
       </c>
-      <c r="B150" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H150,4,FALSE)+23</f>
+      <c r="B150">
         <v>-17.694000000000003</v>
       </c>
     </row>
@@ -1713,8 +1564,7 @@
       <c r="A151">
         <v>148</v>
       </c>
-      <c r="B151" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H151,4,FALSE)+23</f>
+      <c r="B151">
         <v>-17.856000000000002</v>
       </c>
     </row>
@@ -1722,8 +1572,7 @@
       <c r="A152">
         <v>149</v>
       </c>
-      <c r="B152" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H152,4,FALSE)+23</f>
+      <c r="B152">
         <v>-17.962000000000003</v>
       </c>
     </row>
@@ -1731,8 +1580,7 @@
       <c r="A153">
         <v>150</v>
       </c>
-      <c r="B153" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H153,4,FALSE)+23</f>
+      <c r="B153">
         <v>-18</v>
       </c>
     </row>
@@ -1740,8 +1588,7 @@
       <c r="A154">
         <v>151</v>
       </c>
-      <c r="B154" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H154,4,FALSE)+23</f>
+      <c r="B154">
         <v>-17.887999999999998</v>
       </c>
     </row>
@@ -1749,8 +1596,7 @@
       <c r="A155">
         <v>152</v>
       </c>
-      <c r="B155" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H155,4,FALSE)+23</f>
+      <c r="B155">
         <v>-17.584000000000003</v>
       </c>
     </row>
@@ -1758,8 +1604,7 @@
       <c r="A156">
         <v>153</v>
       </c>
-      <c r="B156" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H156,4,FALSE)+23</f>
+      <c r="B156">
         <v>-17.136000000000003</v>
       </c>
     </row>
@@ -1767,8 +1612,7 @@
       <c r="A157">
         <v>154</v>
       </c>
-      <c r="B157" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H157,4,FALSE)+23</f>
+      <c r="B157">
         <v>-16.591999999999999</v>
       </c>
     </row>
@@ -1776,8 +1620,7 @@
       <c r="A158">
         <v>155</v>
       </c>
-      <c r="B158" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H158,4,FALSE)+23</f>
+      <c r="B158">
         <v>-16</v>
       </c>
     </row>
@@ -1785,8 +1628,7 @@
       <c r="A159">
         <v>156</v>
       </c>
-      <c r="B159" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H159,4,FALSE)+23</f>
+      <c r="B159">
         <v>-15.408000000000001</v>
       </c>
     </row>
@@ -1794,8 +1636,7 @@
       <c r="A160">
         <v>157</v>
       </c>
-      <c r="B160" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H160,4,FALSE)+23</f>
+      <c r="B160">
         <v>-14.863999999999997</v>
       </c>
     </row>
@@ -1803,8 +1644,7 @@
       <c r="A161">
         <v>158</v>
       </c>
-      <c r="B161" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H161,4,FALSE)+23</f>
+      <c r="B161">
         <v>-14.415999999999997</v>
       </c>
     </row>
@@ -1812,8 +1652,7 @@
       <c r="A162">
         <v>159</v>
       </c>
-      <c r="B162" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H162,4,FALSE)+23</f>
+      <c r="B162">
         <v>-14.111999999999995</v>
       </c>
     </row>
@@ -1821,8 +1660,7 @@
       <c r="A163">
         <v>160</v>
       </c>
-      <c r="B163" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H163,4,FALSE)+23</f>
+      <c r="B163">
         <v>-14</v>
       </c>
     </row>
@@ -1830,8 +1668,7 @@
       <c r="A164">
         <v>161</v>
       </c>
-      <c r="B164" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H164,4,FALSE)+23</f>
+      <c r="B164">
         <v>-14.088000000000001</v>
       </c>
     </row>
@@ -1839,8 +1676,7 @@
       <c r="A165">
         <v>162</v>
       </c>
-      <c r="B165" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H165,4,FALSE)+23</f>
+      <c r="B165">
         <v>-14.330666666666666</v>
       </c>
     </row>
@@ -1848,8 +1684,7 @@
       <c r="A166">
         <v>163</v>
       </c>
-      <c r="B166" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H166,4,FALSE)+23</f>
+      <c r="B166">
         <v>-14.695999999999998</v>
       </c>
     </row>
@@ -1857,8 +1692,7 @@
       <c r="A167">
         <v>164</v>
       </c>
-      <c r="B167" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H167,4,FALSE)+23</f>
+      <c r="B167">
         <v>-15.152000000000001</v>
       </c>
     </row>
@@ -1866,8 +1700,7 @@
       <c r="A168">
         <v>165</v>
       </c>
-      <c r="B168" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H168,4,FALSE)+23</f>
+      <c r="B168">
         <v>-15.666666666666664</v>
       </c>
     </row>
@@ -1875,8 +1708,7 @@
       <c r="A169">
         <v>166</v>
       </c>
-      <c r="B169" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H169,4,FALSE)+23</f>
+      <c r="B169">
         <v>-16.207999999999998</v>
       </c>
     </row>
@@ -1884,8 +1716,7 @@
       <c r="A170">
         <v>167</v>
       </c>
-      <c r="B170" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H170,4,FALSE)+23</f>
+      <c r="B170">
         <v>-16.744</v>
       </c>
     </row>
@@ -1893,8 +1724,7 @@
       <c r="A171">
         <v>168</v>
       </c>
-      <c r="B171" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H171,4,FALSE)+23</f>
+      <c r="B171">
         <v>-17.242666666666665</v>
       </c>
     </row>
@@ -1902,8 +1732,7 @@
       <c r="A172">
         <v>169</v>
       </c>
-      <c r="B172" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H172,4,FALSE)+23</f>
+      <c r="B172">
         <v>-17.671999999999997</v>
       </c>
     </row>
@@ -1911,8 +1740,7 @@
       <c r="A173">
         <v>170</v>
       </c>
-      <c r="B173" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H173,4,FALSE)+23</f>
+      <c r="B173">
         <v>-18</v>
       </c>
     </row>
@@ -1920,8 +1748,7 @@
       <c r="A174">
         <v>171</v>
       </c>
-      <c r="B174" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H174,4,FALSE)+23</f>
+      <c r="B174">
         <v>-18.271999999999998</v>
       </c>
     </row>
@@ -1929,8 +1756,7 @@
       <c r="A175">
         <v>172</v>
       </c>
-      <c r="B175" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H175,4,FALSE)+23</f>
+      <c r="B175">
         <v>-18.549333333333337</v>
       </c>
     </row>
@@ -1938,8 +1764,7 @@
       <c r="A176">
         <v>173</v>
       </c>
-      <c r="B176" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H176,4,FALSE)+23</f>
+      <c r="B176">
         <v>-18.823999999999998</v>
       </c>
     </row>
@@ -1947,8 +1772,7 @@
       <c r="A177">
         <v>174</v>
       </c>
-      <c r="B177" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H177,4,FALSE)+23</f>
+      <c r="B177">
         <v>-19.088000000000001</v>
       </c>
     </row>
@@ -1956,8 +1780,7 @@
       <c r="A178">
         <v>175</v>
       </c>
-      <c r="B178" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H178,4,FALSE)+23</f>
+      <c r="B178">
         <v>-19.333333333333336</v>
       </c>
     </row>
@@ -1965,8 +1788,7 @@
       <c r="A179">
         <v>176</v>
       </c>
-      <c r="B179" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H179,4,FALSE)+23</f>
+      <c r="B179">
         <v>-19.552</v>
       </c>
     </row>
@@ -1974,8 +1796,7 @@
       <c r="A180">
         <v>177</v>
       </c>
-      <c r="B180" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H180,4,FALSE)+23</f>
+      <c r="B180">
         <v>-19.735999999999997</v>
       </c>
     </row>
@@ -1983,8 +1804,7 @@
       <c r="A181">
         <v>178</v>
       </c>
-      <c r="B181" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H181,4,FALSE)+23</f>
+      <c r="B181">
         <v>-19.877333333333333</v>
       </c>
     </row>
@@ -1992,8 +1812,7 @@
       <c r="A182">
         <v>179</v>
       </c>
-      <c r="B182" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H182,4,FALSE)+23</f>
+      <c r="B182">
         <v>-19.968000000000004</v>
       </c>
     </row>
@@ -2001,8 +1820,7 @@
       <c r="A183">
         <v>180</v>
       </c>
-      <c r="B183" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H183,4,FALSE)+23</f>
+      <c r="B183">
         <v>-20</v>
       </c>
     </row>
@@ -2010,8 +1828,7 @@
       <c r="A184">
         <v>181</v>
       </c>
-      <c r="B184" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H184,4,FALSE)+23</f>
+      <c r="B184">
         <v>-19.887999999999998</v>
       </c>
     </row>
@@ -2019,8 +1836,7 @@
       <c r="A185">
         <v>182</v>
       </c>
-      <c r="B185" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H185,4,FALSE)+23</f>
+      <c r="B185">
         <v>-19.584000000000003</v>
       </c>
     </row>
@@ -2028,8 +1844,7 @@
       <c r="A186">
         <v>183</v>
       </c>
-      <c r="B186" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H186,4,FALSE)+23</f>
+      <c r="B186">
         <v>-19.136000000000003</v>
       </c>
     </row>
@@ -2037,8 +1852,7 @@
       <c r="A187">
         <v>184</v>
       </c>
-      <c r="B187" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H187,4,FALSE)+23</f>
+      <c r="B187">
         <v>-18.591999999999999</v>
       </c>
     </row>
@@ -2046,8 +1860,7 @@
       <c r="A188">
         <v>185</v>
       </c>
-      <c r="B188" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H188,4,FALSE)+23</f>
+      <c r="B188">
         <v>-18</v>
       </c>
     </row>
@@ -2055,8 +1868,7 @@
       <c r="A189">
         <v>186</v>
       </c>
-      <c r="B189" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H189,4,FALSE)+23</f>
+      <c r="B189">
         <v>-17.408000000000001</v>
       </c>
     </row>
@@ -2064,8 +1876,7 @@
       <c r="A190">
         <v>187</v>
       </c>
-      <c r="B190" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H190,4,FALSE)+23</f>
+      <c r="B190">
         <v>-16.863999999999997</v>
       </c>
     </row>
@@ -2073,8 +1884,7 @@
       <c r="A191">
         <v>188</v>
       </c>
-      <c r="B191" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H191,4,FALSE)+23</f>
+      <c r="B191">
         <v>-16.415999999999997</v>
       </c>
     </row>
@@ -2082,8 +1892,7 @@
       <c r="A192">
         <v>189</v>
       </c>
-      <c r="B192" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H192,4,FALSE)+23</f>
+      <c r="B192">
         <v>-16.111999999999995</v>
       </c>
     </row>
@@ -2091,8 +1900,7 @@
       <c r="A193">
         <v>190</v>
       </c>
-      <c r="B193" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H193,4,FALSE)+23</f>
+      <c r="B193">
         <v>-16</v>
       </c>
     </row>
@@ -2100,8 +1908,7 @@
       <c r="A194">
         <v>191</v>
       </c>
-      <c r="B194" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H194,4,FALSE)+23</f>
+      <c r="B194">
         <v>-16</v>
       </c>
     </row>
@@ -2109,8 +1916,7 @@
       <c r="A195">
         <v>192</v>
       </c>
-      <c r="B195" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H195,4,FALSE)+23</f>
+      <c r="B195">
         <v>-16</v>
       </c>
     </row>
@@ -2118,8 +1924,7 @@
       <c r="A196">
         <v>193</v>
       </c>
-      <c r="B196" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H196,4,FALSE)+23</f>
+      <c r="B196">
         <v>-16</v>
       </c>
     </row>
@@ -2127,8 +1932,7 @@
       <c r="A197">
         <v>194</v>
       </c>
-      <c r="B197" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H197,4,FALSE)+23</f>
+      <c r="B197">
         <v>-16</v>
       </c>
     </row>
@@ -2136,8 +1940,7 @@
       <c r="A198">
         <v>195</v>
       </c>
-      <c r="B198" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H198,4,FALSE)+23</f>
+      <c r="B198">
         <v>-16</v>
       </c>
     </row>
@@ -2145,8 +1948,7 @@
       <c r="A199">
         <v>196</v>
       </c>
-      <c r="B199" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H199,4,FALSE)+23</f>
+      <c r="B199">
         <v>-16</v>
       </c>
     </row>
@@ -2154,8 +1956,7 @@
       <c r="A200">
         <v>197</v>
       </c>
-      <c r="B200" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H200,4,FALSE)+23</f>
+      <c r="B200">
         <v>-16</v>
       </c>
     </row>
@@ -2163,8 +1964,7 @@
       <c r="A201">
         <v>198</v>
       </c>
-      <c r="B201" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H201,4,FALSE)+23</f>
+      <c r="B201">
         <v>-16</v>
       </c>
     </row>
@@ -2172,8 +1972,7 @@
       <c r="A202">
         <v>199</v>
       </c>
-      <c r="B202" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H202,4,FALSE)+23</f>
+      <c r="B202">
         <v>-16</v>
       </c>
     </row>
@@ -2181,8 +1980,7 @@
       <c r="A203">
         <v>200</v>
       </c>
-      <c r="B203" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H203,4,FALSE)+23</f>
+      <c r="B203">
         <v>-16</v>
       </c>
     </row>
@@ -2190,8 +1988,7 @@
       <c r="A204">
         <v>201</v>
       </c>
-      <c r="B204" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H204,4,FALSE)+23</f>
+      <c r="B204">
         <v>-16</v>
       </c>
     </row>
@@ -2199,8 +1996,7 @@
       <c r="A205">
         <v>202</v>
       </c>
-      <c r="B205" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H205,4,FALSE)+23</f>
+      <c r="B205">
         <v>-16</v>
       </c>
     </row>
@@ -2208,8 +2004,7 @@
       <c r="A206">
         <v>203</v>
       </c>
-      <c r="B206" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H206,4,FALSE)+23</f>
+      <c r="B206">
         <v>-16</v>
       </c>
     </row>
@@ -2217,8 +2012,7 @@
       <c r="A207">
         <v>204</v>
       </c>
-      <c r="B207" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H207,4,FALSE)+23</f>
+      <c r="B207">
         <v>-16</v>
       </c>
     </row>
@@ -2226,8 +2020,7 @@
       <c r="A208">
         <v>205</v>
       </c>
-      <c r="B208" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H208,4,FALSE)+23</f>
+      <c r="B208">
         <v>-16</v>
       </c>
     </row>
@@ -2235,8 +2028,7 @@
       <c r="A209">
         <v>206</v>
       </c>
-      <c r="B209" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H209,4,FALSE)+23</f>
+      <c r="B209">
         <v>-16</v>
       </c>
     </row>
@@ -2244,8 +2036,7 @@
       <c r="A210">
         <v>207</v>
       </c>
-      <c r="B210" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H210,4,FALSE)+23</f>
+      <c r="B210">
         <v>-16</v>
       </c>
     </row>
@@ -2253,8 +2044,7 @@
       <c r="A211">
         <v>208</v>
       </c>
-      <c r="B211" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H211,4,FALSE)+23</f>
+      <c r="B211">
         <v>-16</v>
       </c>
     </row>
@@ -2262,8 +2052,7 @@
       <c r="A212">
         <v>209</v>
       </c>
-      <c r="B212" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H212,4,FALSE)+23</f>
+      <c r="B212">
         <v>-16</v>
       </c>
     </row>
@@ -2271,8 +2060,7 @@
       <c r="A213">
         <v>210</v>
       </c>
-      <c r="B213" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H213,4,FALSE)+23</f>
+      <c r="B213">
         <v>-16</v>
       </c>
     </row>
@@ -2280,8 +2068,7 @@
       <c r="A214">
         <v>211</v>
       </c>
-      <c r="B214" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H214,4,FALSE)+23</f>
+      <c r="B214">
         <v>-15.962000000000003</v>
       </c>
     </row>
@@ -2289,8 +2076,7 @@
       <c r="A215">
         <v>212</v>
       </c>
-      <c r="B215" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H215,4,FALSE)+23</f>
+      <c r="B215">
         <v>-15.856000000000002</v>
       </c>
     </row>
@@ -2298,8 +2084,7 @@
       <c r="A216">
         <v>213</v>
       </c>
-      <c r="B216" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H216,4,FALSE)+23</f>
+      <c r="B216">
         <v>-15.694000000000003</v>
       </c>
     </row>
@@ -2307,8 +2092,7 @@
       <c r="A217">
         <v>214</v>
       </c>
-      <c r="B217" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H217,4,FALSE)+23</f>
+      <c r="B217">
         <v>-15.488</v>
       </c>
     </row>
@@ -2316,8 +2100,7 @@
       <c r="A218">
         <v>215</v>
       </c>
-      <c r="B218" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H218,4,FALSE)+23</f>
+      <c r="B218">
         <v>-15.25</v>
       </c>
     </row>
@@ -2325,8 +2108,7 @@
       <c r="A219">
         <v>216</v>
       </c>
-      <c r="B219" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H219,4,FALSE)+23</f>
+      <c r="B219">
         <v>-14.991999999999997</v>
       </c>
     </row>
@@ -2334,8 +2116,7 @@
       <c r="A220">
         <v>217</v>
       </c>
-      <c r="B220" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H220,4,FALSE)+23</f>
+      <c r="B220">
         <v>-14.725999999999999</v>
       </c>
     </row>
@@ -2343,8 +2124,7 @@
       <c r="A221">
         <v>218</v>
       </c>
-      <c r="B221" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H221,4,FALSE)+23</f>
+      <c r="B221">
         <v>-14.463999999999999</v>
       </c>
     </row>
@@ -2352,8 +2132,7 @@
       <c r="A222">
         <v>219</v>
       </c>
-      <c r="B222" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H222,4,FALSE)+23</f>
+      <c r="B222">
         <v>-14.217999999999996</v>
       </c>
     </row>
@@ -2361,8 +2140,7 @@
       <c r="A223">
         <v>220</v>
       </c>
-      <c r="B223" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H223,4,FALSE)+23</f>
+      <c r="B223">
         <v>-14</v>
       </c>
     </row>
@@ -2370,8 +2148,7 @@
       <c r="A224">
         <v>221</v>
       </c>
-      <c r="B224" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H224,4,FALSE)+23</f>
+      <c r="B224">
         <v>-13.781999999999996</v>
       </c>
     </row>
@@ -2379,8 +2156,7 @@
       <c r="A225">
         <v>222</v>
       </c>
-      <c r="B225" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H225,4,FALSE)+23</f>
+      <c r="B225">
         <v>-13.536000000000001</v>
       </c>
     </row>
@@ -2388,8 +2164,7 @@
       <c r="A226">
         <v>223</v>
       </c>
-      <c r="B226" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H226,4,FALSE)+23</f>
+      <c r="B226">
         <v>-13.274000000000001</v>
       </c>
     </row>
@@ -2397,8 +2172,7 @@
       <c r="A227">
         <v>224</v>
       </c>
-      <c r="B227" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H227,4,FALSE)+23</f>
+      <c r="B227">
         <v>-13.008000000000003</v>
       </c>
     </row>
@@ -2406,8 +2180,7 @@
       <c r="A228">
         <v>225</v>
       </c>
-      <c r="B228" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H228,4,FALSE)+23</f>
+      <c r="B228">
         <v>-12.75</v>
       </c>
     </row>
@@ -2415,8 +2188,7 @@
       <c r="A229">
         <v>226</v>
       </c>
-      <c r="B229" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H229,4,FALSE)+23</f>
+      <c r="B229">
         <v>-12.512</v>
       </c>
     </row>
@@ -2424,8 +2196,7 @@
       <c r="A230">
         <v>227</v>
       </c>
-      <c r="B230" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H230,4,FALSE)+23</f>
+      <c r="B230">
         <v>-12.305999999999997</v>
       </c>
     </row>
@@ -2433,8 +2204,7 @@
       <c r="A231">
         <v>228</v>
       </c>
-      <c r="B231" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H231,4,FALSE)+23</f>
+      <c r="B231">
         <v>-12.143999999999998</v>
       </c>
     </row>
@@ -2442,8 +2212,7 @@
       <c r="A232">
         <v>229</v>
       </c>
-      <c r="B232" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H232,4,FALSE)+23</f>
+      <c r="B232">
         <v>-12.037999999999997</v>
       </c>
     </row>
@@ -2451,8 +2220,7 @@
       <c r="A233">
         <v>230</v>
       </c>
-      <c r="B233" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H233,4,FALSE)+23</f>
+      <c r="B233">
         <v>-12</v>
       </c>
     </row>
@@ -2460,8 +2228,7 @@
       <c r="A234">
         <v>231</v>
       </c>
-      <c r="B234" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H234,4,FALSE)+23</f>
+      <c r="B234">
         <v>-12.088000000000001</v>
       </c>
     </row>
@@ -2469,8 +2236,7 @@
       <c r="A235">
         <v>232</v>
       </c>
-      <c r="B235" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H235,4,FALSE)+23</f>
+      <c r="B235">
         <v>-12.330666666666666</v>
       </c>
     </row>
@@ -2478,8 +2244,7 @@
       <c r="A236">
         <v>233</v>
       </c>
-      <c r="B236" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H236,4,FALSE)+23</f>
+      <c r="B236">
         <v>-12.695999999999998</v>
       </c>
     </row>
@@ -2487,8 +2252,7 @@
       <c r="A237">
         <v>234</v>
       </c>
-      <c r="B237" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H237,4,FALSE)+23</f>
+      <c r="B237">
         <v>-13.152000000000001</v>
       </c>
     </row>
@@ -2496,8 +2260,7 @@
       <c r="A238">
         <v>235</v>
       </c>
-      <c r="B238" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H238,4,FALSE)+23</f>
+      <c r="B238">
         <v>-13.666666666666664</v>
       </c>
     </row>
@@ -2505,8 +2268,7 @@
       <c r="A239">
         <v>236</v>
       </c>
-      <c r="B239" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H239,4,FALSE)+23</f>
+      <c r="B239">
         <v>-14.207999999999998</v>
       </c>
     </row>
@@ -2514,8 +2276,7 @@
       <c r="A240">
         <v>237</v>
       </c>
-      <c r="B240" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H240,4,FALSE)+23</f>
+      <c r="B240">
         <v>-14.744</v>
       </c>
     </row>
@@ -2523,8 +2284,7 @@
       <c r="A241">
         <v>238</v>
       </c>
-      <c r="B241" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H241,4,FALSE)+23</f>
+      <c r="B241">
         <v>-15.242666666666665</v>
       </c>
     </row>
@@ -2532,8 +2292,7 @@
       <c r="A242">
         <v>239</v>
       </c>
-      <c r="B242" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H242,4,FALSE)+23</f>
+      <c r="B242">
         <v>-15.671999999999997</v>
       </c>
     </row>
@@ -2541,8 +2300,7 @@
       <c r="A243">
         <v>240</v>
       </c>
-      <c r="B243" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H243,4,FALSE)+23</f>
+      <c r="B243">
         <v>-16</v>
       </c>
     </row>
@@ -2550,8 +2308,7 @@
       <c r="A244">
         <v>241</v>
       </c>
-      <c r="B244" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H244,4,FALSE)+23</f>
+      <c r="B244">
         <v>-16.253999999999998</v>
       </c>
     </row>
@@ -2559,8 +2316,7 @@
       <c r="A245">
         <v>242</v>
       </c>
-      <c r="B245" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H245,4,FALSE)+23</f>
+      <c r="B245">
         <v>-16.485333333333337</v>
       </c>
     </row>
@@ -2568,8 +2324,7 @@
       <c r="A246">
         <v>243</v>
       </c>
-      <c r="B246" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H246,4,FALSE)+23</f>
+      <c r="B246">
         <v>-16.698</v>
       </c>
     </row>
@@ -2577,8 +2332,7 @@
       <c r="A247">
         <v>244</v>
       </c>
-      <c r="B247" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H247,4,FALSE)+23</f>
+      <c r="B247">
         <v>-16.896000000000001</v>
       </c>
     </row>
@@ -2586,8 +2340,7 @@
       <c r="A248">
         <v>245</v>
       </c>
-      <c r="B248" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H248,4,FALSE)+23</f>
+      <c r="B248">
         <v>-17.083333333333336</v>
       </c>
     </row>
@@ -2595,8 +2348,7 @@
       <c r="A249">
         <v>246</v>
       </c>
-      <c r="B249" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H249,4,FALSE)+23</f>
+      <c r="B249">
         <v>-17.264000000000003</v>
       </c>
     </row>
@@ -2604,8 +2356,7 @@
       <c r="A250">
         <v>247</v>
       </c>
-      <c r="B250" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H250,4,FALSE)+23</f>
+      <c r="B250">
         <v>-17.442</v>
       </c>
     </row>
@@ -2613,8 +2364,7 @@
       <c r="A251">
         <v>248</v>
       </c>
-      <c r="B251" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H251,4,FALSE)+23</f>
+      <c r="B251">
         <v>-17.621333333333332</v>
       </c>
     </row>
@@ -2622,8 +2372,7 @@
       <c r="A252">
         <v>249</v>
       </c>
-      <c r="B252" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H252,4,FALSE)+23</f>
+      <c r="B252">
         <v>-17.805999999999997</v>
       </c>
     </row>
@@ -2631,8 +2380,7 @@
       <c r="A253">
         <v>250</v>
       </c>
-      <c r="B253" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H253,4,FALSE)+23</f>
+      <c r="B253">
         <v>-18</v>
       </c>
     </row>
@@ -2640,8 +2388,7 @@
       <c r="A254">
         <v>251</v>
       </c>
-      <c r="B254" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H254,4,FALSE)+23</f>
+      <c r="B254">
         <v>-18.200000000000003</v>
       </c>
     </row>
@@ -2649,8 +2396,7 @@
       <c r="A255">
         <v>252</v>
       </c>
-      <c r="B255" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H255,4,FALSE)+23</f>
+      <c r="B255">
         <v>-18.399999999999999</v>
       </c>
     </row>
@@ -2658,8 +2404,7 @@
       <c r="A256">
         <v>253</v>
       </c>
-      <c r="B256" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H256,4,FALSE)+23</f>
+      <c r="B256">
         <v>-18.600000000000001</v>
       </c>
     </row>
@@ -2667,8 +2412,7 @@
       <c r="A257">
         <v>254</v>
       </c>
-      <c r="B257" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H257,4,FALSE)+23</f>
+      <c r="B257">
         <v>-18.799999999999997</v>
       </c>
     </row>
@@ -2676,8 +2420,7 @@
       <c r="A258">
         <v>255</v>
       </c>
-      <c r="B258" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H258,4,FALSE)+23</f>
+      <c r="B258">
         <v>-19</v>
       </c>
     </row>
@@ -2685,8 +2428,7 @@
       <c r="A259">
         <v>256</v>
       </c>
-      <c r="B259" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H259,4,FALSE)+23</f>
+      <c r="B259">
         <v>-19.200000000000003</v>
       </c>
     </row>
@@ -2694,8 +2436,7 @@
       <c r="A260">
         <v>257</v>
       </c>
-      <c r="B260" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H260,4,FALSE)+23</f>
+      <c r="B260">
         <v>-19.399999999999999</v>
       </c>
     </row>
@@ -2703,8 +2444,7 @@
       <c r="A261">
         <v>258</v>
       </c>
-      <c r="B261" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H261,4,FALSE)+23</f>
+      <c r="B261">
         <v>-19.600000000000001</v>
       </c>
     </row>
@@ -2712,8 +2452,7 @@
       <c r="A262">
         <v>259</v>
       </c>
-      <c r="B262" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H262,4,FALSE)+23</f>
+      <c r="B262">
         <v>-19.799999999999997</v>
       </c>
     </row>
@@ -2721,8 +2460,7 @@
       <c r="A263">
         <v>260</v>
       </c>
-      <c r="B263" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H263,4,FALSE)+23</f>
+      <c r="B263">
         <v>-20</v>
       </c>
     </row>
@@ -2730,8 +2468,7 @@
       <c r="A264">
         <v>261</v>
       </c>
-      <c r="B264" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H264,4,FALSE)+23</f>
+      <c r="B264">
         <v>-20.218000000000004</v>
       </c>
     </row>
@@ -2739,8 +2476,7 @@
       <c r="A265">
         <v>262</v>
       </c>
-      <c r="B265" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H265,4,FALSE)+23</f>
+      <c r="B265">
         <v>-20.463999999999999</v>
       </c>
     </row>
@@ -2748,8 +2484,7 @@
       <c r="A266">
         <v>263</v>
       </c>
-      <c r="B266" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H266,4,FALSE)+23</f>
+      <c r="B266">
         <v>-20.725999999999999</v>
       </c>
     </row>
@@ -2757,8 +2492,7 @@
       <c r="A267">
         <v>264</v>
       </c>
-      <c r="B267" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H267,4,FALSE)+23</f>
+      <c r="B267">
         <v>-20.991999999999997</v>
       </c>
     </row>
@@ -2766,8 +2500,7 @@
       <c r="A268">
         <v>265</v>
       </c>
-      <c r="B268" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H268,4,FALSE)+23</f>
+      <c r="B268">
         <v>-21.25</v>
       </c>
     </row>
@@ -2775,8 +2508,7 @@
       <c r="A269">
         <v>266</v>
       </c>
-      <c r="B269" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H269,4,FALSE)+23</f>
+      <c r="B269">
         <v>-21.488</v>
       </c>
     </row>
@@ -2784,8 +2516,7 @@
       <c r="A270">
         <v>267</v>
       </c>
-      <c r="B270" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H270,4,FALSE)+23</f>
+      <c r="B270">
         <v>-21.694000000000003</v>
       </c>
     </row>
@@ -2793,8 +2524,7 @@
       <c r="A271">
         <v>268</v>
       </c>
-      <c r="B271" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H271,4,FALSE)+23</f>
+      <c r="B271">
         <v>-21.856000000000002</v>
       </c>
     </row>
@@ -2802,8 +2532,7 @@
       <c r="A272">
         <v>269</v>
       </c>
-      <c r="B272" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H272,4,FALSE)+23</f>
+      <c r="B272">
         <v>-21.962000000000003</v>
       </c>
     </row>
@@ -2811,8 +2540,7 @@
       <c r="A273">
         <v>270</v>
       </c>
-      <c r="B273" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H273,4,FALSE)+23</f>
+      <c r="B273">
         <v>-22</v>
       </c>
     </row>
@@ -2820,8 +2548,7 @@
       <c r="A274">
         <v>271</v>
       </c>
-      <c r="B274" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H274,4,FALSE)+23</f>
+      <c r="B274">
         <v>-21.939428571428572</v>
       </c>
     </row>
@@ -2829,8 +2556,7 @@
       <c r="A275">
         <v>272</v>
       </c>
-      <c r="B275" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H275,4,FALSE)+23</f>
+      <c r="B275">
         <v>-21.766857142857141</v>
       </c>
     </row>
@@ -2838,8 +2564,7 @@
       <c r="A276">
         <v>273</v>
       </c>
-      <c r="B276" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H276,4,FALSE)+23</f>
+      <c r="B276">
         <v>-21.496000000000002</v>
       </c>
     </row>
@@ -2847,8 +2572,7 @@
       <c r="A277">
         <v>274</v>
       </c>
-      <c r="B277" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H277,4,FALSE)+23</f>
+      <c r="B277">
         <v>-21.140571428571427</v>
       </c>
     </row>
@@ -2856,8 +2580,7 @@
       <c r="A278">
         <v>275</v>
       </c>
-      <c r="B278" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H278,4,FALSE)+23</f>
+      <c r="B278">
         <v>-20.714285714285715</v>
       </c>
     </row>
@@ -2865,8 +2588,7 @@
       <c r="A279">
         <v>276</v>
       </c>
-      <c r="B279" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H279,4,FALSE)+23</f>
+      <c r="B279">
         <v>-20.23085714285714</v>
       </c>
     </row>
@@ -2874,8 +2596,7 @@
       <c r="A280">
         <v>277</v>
       </c>
-      <c r="B280" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H280,4,FALSE)+23</f>
+      <c r="B280">
         <v>-19.704000000000001</v>
       </c>
     </row>
@@ -2883,8 +2604,7 @@
       <c r="A281">
         <v>278</v>
       </c>
-      <c r="B281" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H281,4,FALSE)+23</f>
+      <c r="B281">
         <v>-19.14742857142857</v>
       </c>
     </row>
@@ -2892,8 +2612,7 @@
       <c r="A282">
         <v>279</v>
       </c>
-      <c r="B282" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H282,4,FALSE)+23</f>
+      <c r="B282">
         <v>-18.574857142857141</v>
       </c>
     </row>
@@ -2901,8 +2620,7 @@
       <c r="A283">
         <v>280</v>
       </c>
-      <c r="B283" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H283,4,FALSE)+23</f>
+      <c r="B283">
         <v>-18</v>
       </c>
     </row>
@@ -2910,8 +2628,7 @@
       <c r="A284">
         <v>281</v>
       </c>
-      <c r="B284" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H284,4,FALSE)+23</f>
+      <c r="B284">
         <v>-17.287142857142854</v>
       </c>
     </row>
@@ -2919,8 +2636,7 @@
       <c r="A285">
         <v>282</v>
       </c>
-      <c r="B285" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H285,4,FALSE)+23</f>
+      <c r="B285">
         <v>-16.335238095238097</v>
       </c>
     </row>
@@ -2928,8 +2644,7 @@
       <c r="A286">
         <v>283</v>
       </c>
-      <c r="B286" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H286,4,FALSE)+23</f>
+      <c r="B286">
         <v>-15.21</v>
       </c>
     </row>
@@ -2937,8 +2652,7 @@
       <c r="A287">
         <v>284</v>
       </c>
-      <c r="B287" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H287,4,FALSE)+23</f>
+      <c r="B287">
         <v>-13.977142857142859</v>
       </c>
     </row>
@@ -2946,8 +2660,7 @@
       <c r="A288">
         <v>285</v>
       </c>
-      <c r="B288" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H288,4,FALSE)+23</f>
+      <c r="B288">
         <v>-12.702380952380956</v>
       </c>
     </row>
@@ -2955,8 +2668,7 @@
       <c r="A289">
         <v>286</v>
       </c>
-      <c r="B289" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H289,4,FALSE)+23</f>
+      <c r="B289">
         <v>-11.451428571428572</v>
       </c>
     </row>
@@ -2964,8 +2676,7 @@
       <c r="A290">
         <v>287</v>
       </c>
-      <c r="B290" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H290,4,FALSE)+23</f>
+      <c r="B290">
         <v>-10.29</v>
       </c>
     </row>
@@ -2973,8 +2684,7 @@
       <c r="A291">
         <v>288</v>
       </c>
-      <c r="B291" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H291,4,FALSE)+23</f>
+      <c r="B291">
         <v>-9.2838095238095235</v>
       </c>
     </row>
@@ -2982,8 +2692,7 @@
       <c r="A292">
         <v>289</v>
       </c>
-      <c r="B292" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H292,4,FALSE)+23</f>
+      <c r="B292">
         <v>-8.4985714285714309</v>
       </c>
     </row>
@@ -2991,8 +2700,7 @@
       <c r="A293">
         <v>290</v>
       </c>
-      <c r="B293" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H293,4,FALSE)+23</f>
+      <c r="B293">
         <v>-8</v>
       </c>
     </row>
@@ -3000,8 +2708,7 @@
       <c r="A294">
         <v>291</v>
       </c>
-      <c r="B294" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H294,4,FALSE)+23</f>
+      <c r="B294">
         <v>-7.6920000000000002</v>
       </c>
     </row>
@@ -3009,8 +2716,7 @@
       <c r="A295">
         <v>292</v>
       </c>
-      <c r="B295" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H295,4,FALSE)+23</f>
+      <c r="B295">
         <v>-7.4293333333333322</v>
       </c>
     </row>
@@ -3018,8 +2724,7 @@
       <c r="A296">
         <v>293</v>
       </c>
-      <c r="B296" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H296,4,FALSE)+23</f>
+      <c r="B296">
         <v>-7.2040000000000006</v>
       </c>
     </row>
@@ -3027,8 +2732,7 @@
       <c r="A297">
         <v>294</v>
       </c>
-      <c r="B297" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H297,4,FALSE)+23</f>
+      <c r="B297">
         <v>-7.0079999999999991</v>
       </c>
     </row>
@@ -3036,8 +2740,7 @@
       <c r="A298">
         <v>295</v>
       </c>
-      <c r="B298" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H298,4,FALSE)+23</f>
+      <c r="B298">
         <v>-6.8333333333333321</v>
       </c>
     </row>
@@ -3045,8 +2748,7 @@
       <c r="A299">
         <v>296</v>
       </c>
-      <c r="B299" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H299,4,FALSE)+23</f>
+      <c r="B299">
         <v>-6.6720000000000006</v>
       </c>
     </row>
@@ -3054,8 +2756,7 @@
       <c r="A300">
         <v>297</v>
       </c>
-      <c r="B300" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H300,4,FALSE)+23</f>
+      <c r="B300">
         <v>-6.5159999999999982</v>
       </c>
     </row>
@@ -3063,8 +2764,7 @@
       <c r="A301">
         <v>298</v>
       </c>
-      <c r="B301" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H301,4,FALSE)+23</f>
+      <c r="B301">
         <v>-6.3573333333333331</v>
       </c>
     </row>
@@ -3072,8 +2772,7 @@
       <c r="A302">
         <v>299</v>
       </c>
-      <c r="B302" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H302,4,FALSE)+23</f>
+      <c r="B302">
         <v>-6.1879999999999988</v>
       </c>
     </row>
@@ -3081,8 +2780,7 @@
       <c r="A303">
         <v>300</v>
       </c>
-      <c r="B303" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H303,4,FALSE)+23</f>
+      <c r="B303">
         <v>-6</v>
       </c>
     </row>
@@ -3090,8 +2788,7 @@
       <c r="A304">
         <v>301</v>
       </c>
-      <c r="B304" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H304,4,FALSE)+23</f>
+      <c r="B304">
         <v>-5.8000000000000007</v>
       </c>
     </row>
@@ -3099,8 +2796,7 @@
       <c r="A305">
         <v>302</v>
       </c>
-      <c r="B305" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H305,4,FALSE)+23</f>
+      <c r="B305">
         <v>-5.6000000000000014</v>
       </c>
     </row>
@@ -3108,8 +2804,7 @@
       <c r="A306">
         <v>303</v>
       </c>
-      <c r="B306" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H306,4,FALSE)+23</f>
+      <c r="B306">
         <v>-5.3999999999999986</v>
       </c>
     </row>
@@ -3117,8 +2812,7 @@
       <c r="A307">
         <v>304</v>
       </c>
-      <c r="B307" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H307,4,FALSE)+23</f>
+      <c r="B307">
         <v>-5.1999999999999993</v>
       </c>
     </row>
@@ -3126,8 +2820,7 @@
       <c r="A308">
         <v>305</v>
       </c>
-      <c r="B308" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H308,4,FALSE)+23</f>
+      <c r="B308">
         <v>-5</v>
       </c>
     </row>
@@ -3135,8 +2828,7 @@
       <c r="A309">
         <v>306</v>
       </c>
-      <c r="B309" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H309,4,FALSE)+23</f>
+      <c r="B309">
         <v>-4.8000000000000007</v>
       </c>
     </row>
@@ -3144,8 +2836,7 @@
       <c r="A310">
         <v>307</v>
       </c>
-      <c r="B310" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H310,4,FALSE)+23</f>
+      <c r="B310">
         <v>-4.6000000000000014</v>
       </c>
     </row>
@@ -3153,8 +2844,7 @@
       <c r="A311">
         <v>308</v>
       </c>
-      <c r="B311" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H311,4,FALSE)+23</f>
+      <c r="B311">
         <v>-4.3999999999999986</v>
       </c>
     </row>
@@ -3162,8 +2852,7 @@
       <c r="A312">
         <v>309</v>
       </c>
-      <c r="B312" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H312,4,FALSE)+23</f>
+      <c r="B312">
         <v>-4.1999999999999993</v>
       </c>
     </row>
@@ -3171,8 +2860,7 @@
       <c r="A313">
         <v>310</v>
       </c>
-      <c r="B313" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H313,4,FALSE)+23</f>
+      <c r="B313">
         <v>-4</v>
       </c>
     </row>
@@ -3180,8 +2868,7 @@
       <c r="A314">
         <v>311</v>
       </c>
-      <c r="B314" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H314,4,FALSE)+23</f>
+      <c r="B314">
         <v>-3.782</v>
       </c>
     </row>
@@ -3189,8 +2876,7 @@
       <c r="A315">
         <v>312</v>
       </c>
-      <c r="B315" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H315,4,FALSE)+23</f>
+      <c r="B315">
         <v>-3.5360000000000014</v>
       </c>
     </row>
@@ -3198,8 +2884,7 @@
       <c r="A316">
         <v>313</v>
       </c>
-      <c r="B316" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H316,4,FALSE)+23</f>
+      <c r="B316">
         <v>-3.2740000000000009</v>
       </c>
     </row>
@@ -3207,8 +2892,7 @@
       <c r="A317">
         <v>314</v>
       </c>
-      <c r="B317" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H317,4,FALSE)+23</f>
+      <c r="B317">
         <v>-3.0079999999999991</v>
       </c>
     </row>
@@ -3216,8 +2900,7 @@
       <c r="A318">
         <v>315</v>
       </c>
-      <c r="B318" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H318,4,FALSE)+23</f>
+      <c r="B318">
         <v>-2.75</v>
       </c>
     </row>
@@ -3225,8 +2908,7 @@
       <c r="A319">
         <v>316</v>
       </c>
-      <c r="B319" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H319,4,FALSE)+23</f>
+      <c r="B319">
         <v>-2.5120000000000005</v>
       </c>
     </row>
@@ -3234,8 +2916,7 @@
       <c r="A320">
         <v>317</v>
       </c>
-      <c r="B320" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H320,4,FALSE)+23</f>
+      <c r="B320">
         <v>-2.3060000000000009</v>
       </c>
     </row>
@@ -3243,8 +2924,7 @@
       <c r="A321">
         <v>318</v>
       </c>
-      <c r="B321" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H321,4,FALSE)+23</f>
+      <c r="B321">
         <v>-2.1439999999999984</v>
       </c>
     </row>
@@ -3252,8 +2932,7 @@
       <c r="A322">
         <v>319</v>
       </c>
-      <c r="B322" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H322,4,FALSE)+23</f>
+      <c r="B322">
         <v>-2.0380000000000003</v>
       </c>
     </row>
@@ -3261,8 +2940,7 @@
       <c r="A323">
         <v>320</v>
       </c>
-      <c r="B323" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H323,4,FALSE)+23</f>
+      <c r="B323">
         <v>-2</v>
       </c>
     </row>
@@ -3270,8 +2948,7 @@
       <c r="A324">
         <v>321</v>
       </c>
-      <c r="B324" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H324,4,FALSE)+23</f>
+      <c r="B324">
         <v>-2</v>
       </c>
     </row>
@@ -3279,8 +2956,7 @@
       <c r="A325">
         <v>322</v>
       </c>
-      <c r="B325" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H325,4,FALSE)+23</f>
+      <c r="B325">
         <v>-2</v>
       </c>
     </row>
@@ -3288,8 +2964,7 @@
       <c r="A326">
         <v>323</v>
       </c>
-      <c r="B326" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H326,4,FALSE)+23</f>
+      <c r="B326">
         <v>-2</v>
       </c>
     </row>
@@ -3297,8 +2972,7 @@
       <c r="A327">
         <v>324</v>
       </c>
-      <c r="B327" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H327,4,FALSE)+23</f>
+      <c r="B327">
         <v>-2</v>
       </c>
     </row>
@@ -3306,8 +2980,7 @@
       <c r="A328">
         <v>325</v>
       </c>
-      <c r="B328" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H328,4,FALSE)+23</f>
+      <c r="B328">
         <v>-2</v>
       </c>
     </row>
@@ -3315,8 +2988,7 @@
       <c r="A329">
         <v>326</v>
       </c>
-      <c r="B329" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H329,4,FALSE)+23</f>
+      <c r="B329">
         <v>-2</v>
       </c>
     </row>
@@ -3324,8 +2996,7 @@
       <c r="A330">
         <v>327</v>
       </c>
-      <c r="B330" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H330,4,FALSE)+23</f>
+      <c r="B330">
         <v>-2</v>
       </c>
     </row>
@@ -3333,8 +3004,7 @@
       <c r="A331">
         <v>328</v>
       </c>
-      <c r="B331" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H331,4,FALSE)+23</f>
+      <c r="B331">
         <v>-2</v>
       </c>
     </row>
@@ -3342,8 +3012,7 @@
       <c r="A332">
         <v>329</v>
       </c>
-      <c r="B332" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H332,4,FALSE)+23</f>
+      <c r="B332">
         <v>-2</v>
       </c>
     </row>
@@ -3351,8 +3020,7 @@
       <c r="A333">
         <v>330</v>
       </c>
-      <c r="B333" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H333,4,FALSE)+23</f>
+      <c r="B333">
         <v>-2</v>
       </c>
     </row>
@@ -3360,8 +3028,7 @@
       <c r="A334">
         <v>331</v>
       </c>
-      <c r="B334" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H334,4,FALSE)+23</f>
+      <c r="B334">
         <v>-2</v>
       </c>
     </row>
@@ -3369,8 +3036,7 @@
       <c r="A335">
         <v>332</v>
       </c>
-      <c r="B335" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H335,4,FALSE)+23</f>
+      <c r="B335">
         <v>-2</v>
       </c>
     </row>
@@ -3378,8 +3044,7 @@
       <c r="A336">
         <v>333</v>
       </c>
-      <c r="B336" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H336,4,FALSE)+23</f>
+      <c r="B336">
         <v>-2</v>
       </c>
     </row>
@@ -3387,8 +3052,7 @@
       <c r="A337">
         <v>334</v>
       </c>
-      <c r="B337" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H337,4,FALSE)+23</f>
+      <c r="B337">
         <v>-2</v>
       </c>
     </row>
@@ -3396,8 +3060,7 @@
       <c r="A338">
         <v>335</v>
       </c>
-      <c r="B338" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H338,4,FALSE)+23</f>
+      <c r="B338">
         <v>-2</v>
       </c>
     </row>
@@ -3405,8 +3068,7 @@
       <c r="A339">
         <v>336</v>
       </c>
-      <c r="B339" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H339,4,FALSE)+23</f>
+      <c r="B339">
         <v>-2</v>
       </c>
     </row>
@@ -3414,8 +3076,7 @@
       <c r="A340">
         <v>337</v>
       </c>
-      <c r="B340" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H340,4,FALSE)+23</f>
+      <c r="B340">
         <v>-2</v>
       </c>
     </row>
@@ -3423,8 +3084,7 @@
       <c r="A341">
         <v>338</v>
       </c>
-      <c r="B341" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H341,4,FALSE)+23</f>
+      <c r="B341">
         <v>-2</v>
       </c>
     </row>
@@ -3432,8 +3092,7 @@
       <c r="A342">
         <v>339</v>
       </c>
-      <c r="B342" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H342,4,FALSE)+23</f>
+      <c r="B342">
         <v>-2</v>
       </c>
     </row>
@@ -3441,8 +3100,7 @@
       <c r="A343">
         <v>340</v>
       </c>
-      <c r="B343" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H343,4,FALSE)+23</f>
+      <c r="B343">
         <v>-2</v>
       </c>
     </row>
@@ -3450,8 +3108,7 @@
       <c r="A344">
         <v>341</v>
       </c>
-      <c r="B344" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H344,4,FALSE)+23</f>
+      <c r="B344">
         <v>-2</v>
       </c>
     </row>
@@ -3459,8 +3116,7 @@
       <c r="A345">
         <v>342</v>
       </c>
-      <c r="B345" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H345,4,FALSE)+23</f>
+      <c r="B345">
         <v>-2</v>
       </c>
     </row>
@@ -3468,8 +3124,7 @@
       <c r="A346">
         <v>343</v>
       </c>
-      <c r="B346" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H346,4,FALSE)+23</f>
+      <c r="B346">
         <v>-2</v>
       </c>
     </row>
@@ -3477,8 +3132,7 @@
       <c r="A347">
         <v>344</v>
       </c>
-      <c r="B347" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H347,4,FALSE)+23</f>
+      <c r="B347">
         <v>-2</v>
       </c>
     </row>
@@ -3486,8 +3140,7 @@
       <c r="A348">
         <v>345</v>
       </c>
-      <c r="B348" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H348,4,FALSE)+23</f>
+      <c r="B348">
         <v>-2</v>
       </c>
     </row>
@@ -3495,8 +3148,7 @@
       <c r="A349">
         <v>346</v>
       </c>
-      <c r="B349" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H349,4,FALSE)+23</f>
+      <c r="B349">
         <v>-2</v>
       </c>
     </row>
@@ -3504,8 +3156,7 @@
       <c r="A350">
         <v>347</v>
       </c>
-      <c r="B350" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H350,4,FALSE)+23</f>
+      <c r="B350">
         <v>-2</v>
       </c>
     </row>
@@ -3513,8 +3164,7 @@
       <c r="A351">
         <v>348</v>
       </c>
-      <c r="B351" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H351,4,FALSE)+23</f>
+      <c r="B351">
         <v>-2</v>
       </c>
     </row>
@@ -3522,8 +3172,7 @@
       <c r="A352">
         <v>349</v>
       </c>
-      <c r="B352" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H352,4,FALSE)+23</f>
+      <c r="B352">
         <v>-2</v>
       </c>
     </row>
@@ -3531,8 +3180,7 @@
       <c r="A353">
         <v>350</v>
       </c>
-      <c r="B353" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H353,4,FALSE)+23</f>
+      <c r="B353">
         <v>-2</v>
       </c>
     </row>
@@ -3540,8 +3188,7 @@
       <c r="A354">
         <v>351</v>
       </c>
-      <c r="B354" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H354,4,FALSE)+23</f>
+      <c r="B354">
         <v>-1.9710000000000001</v>
       </c>
     </row>
@@ -3549,8 +3196,7 @@
       <c r="A355">
         <v>352</v>
       </c>
-      <c r="B355" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H355,4,FALSE)+23</f>
+      <c r="B355">
         <v>-1.8880000000000017</v>
       </c>
     </row>
@@ -3558,8 +3204,7 @@
       <c r="A356">
         <v>353</v>
       </c>
-      <c r="B356" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H356,4,FALSE)+23</f>
+      <c r="B356">
         <v>-1.7570000000000014</v>
       </c>
     </row>
@@ -3567,8 +3212,7 @@
       <c r="A357">
         <v>354</v>
       </c>
-      <c r="B357" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H357,4,FALSE)+23</f>
+      <c r="B357">
         <v>-1.5839999999999996</v>
       </c>
     </row>
@@ -3576,8 +3220,7 @@
       <c r="A358">
         <v>355</v>
       </c>
-      <c r="B358" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H358,4,FALSE)+23</f>
+      <c r="B358">
         <v>-1.375</v>
       </c>
     </row>
@@ -3585,8 +3228,7 @@
       <c r="A359">
         <v>356</v>
       </c>
-      <c r="B359" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H359,4,FALSE)+23</f>
+      <c r="B359">
         <v>-1.1359999999999992</v>
       </c>
     </row>
@@ -3594,8 +3236,7 @@
       <c r="A360">
         <v>357</v>
       </c>
-      <c r="B360" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H360,4,FALSE)+23</f>
+      <c r="B360">
         <v>-0.87300000000000111</v>
       </c>
     </row>
@@ -3603,8 +3244,7 @@
       <c r="A361">
         <v>358</v>
       </c>
-      <c r="B361" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H361,4,FALSE)+23</f>
+      <c r="B361">
         <v>-0.59199999999999875</v>
       </c>
     </row>
@@ -3612,8 +3252,7 @@
       <c r="A362">
         <v>359</v>
       </c>
-      <c r="B362" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H362,4,FALSE)+23</f>
+      <c r="B362">
         <v>-0.29899999999999949</v>
       </c>
     </row>
@@ -3621,13 +3260,13 @@
       <c r="A363">
         <v>360</v>
       </c>
-      <c r="B363" s="1">
-        <f ca="1">_xll.INTERPOLATE($A$2:$A$38,$B$2:$B$38,$H363,4,FALSE)+23</f>
+      <c r="B363">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>